<commit_message>
Inventar implementiert, Adventure Klasse angelegt
- Adventure Klasse: als Main Klasse, aktuell ist nur Zeug zum testen drin.

- Item Attribute von private zu public geändert

- Item.anschauen() hinzugefügt: gibt Name und Beschreibung aus.

- Spieler:Attribut Inventar von Array zu ArrayList geändert, weil ist einfach besser. (Dynamisch und so.)

- Inventar implementiert, mit Spieler.insInventar(Item) um ein Item hinzuzufügen, und Spieler.liesInventar() um das Inventar direkt printen zu lassen. (sollte man vllt zu "printInventar" oder so umbenennen.

Doku angepasst
</commit_message>
<xml_diff>
--- a/doku/Klassendiagramm.xlsx
+++ b/doku/Klassendiagramm.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125BC784-B2BC-43C3-A792-7C194F2F678D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD92824-0D07-47F7-86AC-B0D640D46CA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Spieler</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Inventar</t>
   </si>
   <si>
-    <t>Item[]</t>
-  </si>
-  <si>
     <t>Ort</t>
   </si>
   <si>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>gibt this.Beschreibung aus</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Item&gt;</t>
+  </si>
+  <si>
+    <t>gibt Name und Beschreibung aus.</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -220,6 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -503,11 +507,12 @@
   <dimension ref="B2:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
@@ -523,15 +528,15 @@
       </c>
       <c r="C2" s="8"/>
       <c r="G2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" s="8"/>
       <c r="L2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" s="8"/>
       <c r="U2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="V2" s="8"/>
     </row>
@@ -540,87 +545,93 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="L4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="U4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="G5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U5" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="V5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="L6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>